<commit_message>
Fixed questions according to manual and not paper
</commit_message>
<xml_diff>
--- a/Tesis/CodeToInspectResults/EvaluaciónIGASCEOrdenada.xlsx
+++ b/Tesis/CodeToInspectResults/EvaluaciónIGASCEOrdenada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alons\Desktop\Godot\Tesis\Thesis-IGACSE\Tesis\CodeToInspectResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alonsout\desktop\tesis\Thesis-IGACSE\Tesis\CodeToInspectResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6E22F9-0EB8-4B38-9445-82B1EC3F5E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D89E68B-7D96-4D09-A1B3-C89931891640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -408,8 +408,30 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +442,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -435,10 +469,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,17 +697,17 @@
   </sheetPr>
   <dimension ref="A4:AN51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.109375" customWidth="1"/>
     <col min="30" max="30" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -772,7 +810,7 @@
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
     </row>
-    <row r="5" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
@@ -873,7 +911,7 @@
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
     </row>
-    <row r="6" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>61</v>
       </c>
@@ -965,7 +1003,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
@@ -1063,7 +1101,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>63</v>
       </c>
@@ -1161,7 +1199,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>61</v>
       </c>
@@ -1259,7 +1297,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
@@ -1354,7 +1392,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>61</v>
       </c>
@@ -1452,7 +1490,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>61</v>
       </c>
@@ -1547,7 +1585,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>61</v>
       </c>
@@ -1645,7 +1683,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
@@ -1743,7 +1781,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>61</v>
       </c>
@@ -1838,7 +1876,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="3:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:40" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1936,7 +1974,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>61</v>
       </c>
@@ -2034,7 +2072,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
@@ -2129,7 +2167,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
@@ -2227,7 +2265,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>63</v>
       </c>
@@ -2313,7 +2351,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -2321,7 +2359,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ref="C22:AE22" si="0">COUNTIF(C$6:C$20, "Muy en desacuerdo")</f>
+        <f t="shared" ref="C22:K22" si="0">COUNTIF(C$6:C$20, "Muy en desacuerdo")</f>
         <v>0</v>
       </c>
       <c r="D22" s="1">
@@ -2357,83 +2395,83 @@
         <v>0</v>
       </c>
       <c r="L22" s="1">
-        <f>COUNTIF(L$6:L$20, "Muy en desacuerdo")</f>
+        <f t="shared" ref="L22:AD22" si="1">COUNTIF(L$6:L$20, "Muy en desacuerdo")</f>
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <f>COUNTIF(M$6:M$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <f>COUNTIF(N$6:N$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O22" s="1">
-        <f>COUNTIF(O$6:O$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P22" s="1">
-        <f>COUNTIF(P$6:P$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q22" s="1">
-        <f>COUNTIF(Q$6:Q$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <f>COUNTIF(R$6:R$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S22" s="1">
-        <f>COUNTIF(S$6:S$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T22" s="1">
-        <f>COUNTIF(T$6:T$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U22" s="1">
-        <f>COUNTIF(U$6:U$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V22" s="1">
-        <f>COUNTIF(V$6:V$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W22" s="1">
-        <f>COUNTIF(W$6:W$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="X22" s="1">
-        <f>COUNTIF(X$6:X$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <f>COUNTIF(Y$6:Y$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z22" s="1">
-        <f>COUNTIF(Z$6:Z$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA22" s="1">
-        <f>COUNTIF(AA$6:AA$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB22" s="1">
-        <f>COUNTIF(AB$6:AB$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC22" s="1">
-        <f>COUNTIF(AC$6:AC$20, "Muy en desacuerdo")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD22" s="1">
-        <f>COUNTIF(AD$6:AD$20, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -2441,119 +2479,119 @@
         <v>67</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ref="C23:AE23" si="1">COUNTIF(C$6:C$20, "En desacuerdo")</f>
+        <f t="shared" ref="C23:K23" si="2">COUNTIF(C$6:C$20, "En desacuerdo")</f>
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L23" s="1">
-        <f>COUNTIF(L$6:L$20, "En desacuerdo")</f>
+        <f t="shared" ref="L23:AD23" si="3">COUNTIF(L$6:L$20, "En desacuerdo")</f>
         <v>1</v>
       </c>
       <c r="M23" s="1">
-        <f>COUNTIF(M$6:M$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f>COUNTIF(N$6:N$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O23" s="1">
-        <f>COUNTIF(O$6:O$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P23" s="1">
-        <f>COUNTIF(P$6:P$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <f>COUNTIF(Q$6:Q$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R23" s="1">
-        <f>COUNTIF(R$6:R$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S23" s="1">
-        <f>COUNTIF(S$6:S$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T23" s="1">
-        <f>COUNTIF(T$6:T$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <f>COUNTIF(U$6:U$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V23" s="1">
-        <f>COUNTIF(V$6:V$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W23" s="1">
-        <f>COUNTIF(W$6:W$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X23" s="1">
-        <f>COUNTIF(X$6:X$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Y23" s="1">
-        <f>COUNTIF(Y$6:Y$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z23" s="1">
-        <f>COUNTIF(Z$6:Z$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA23" s="1">
-        <f>COUNTIF(AA$6:AA$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AB23" s="1">
-        <f>COUNTIF(AB$6:AB$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="AC23" s="1">
-        <f>COUNTIF(AC$6:AC$20, "En desacuerdo")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD23" s="1">
-        <f>COUNTIF(AD$6:AD$20, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -2561,119 +2599,119 @@
         <v>62</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ref="C24:AE24" si="2">COUNTIF(C$6:C$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" ref="C24:K24" si="4">COUNTIF(C$6:C$20, "Ni en desacuerdo ni de acuerdo")</f>
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L24" s="1">
-        <f>COUNTIF(L$6:L$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" ref="L24:AD24" si="5">COUNTIF(L$6:L$20, "Ni en desacuerdo ni de acuerdo")</f>
         <v>2</v>
       </c>
       <c r="M24" s="1">
-        <f>COUNTIF(M$6:M$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N24" s="1">
-        <f>COUNTIF(N$6:N$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O24" s="1">
-        <f>COUNTIF(O$6:O$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P24" s="1">
-        <f>COUNTIF(P$6:P$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q24" s="1">
-        <f>COUNTIF(Q$6:Q$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R24" s="1">
-        <f>COUNTIF(R$6:R$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="S24" s="1">
-        <f>COUNTIF(S$6:S$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="T24" s="1">
-        <f>COUNTIF(T$6:T$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U24" s="1">
-        <f>COUNTIF(U$6:U$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V24" s="1">
-        <f>COUNTIF(V$6:V$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <f>COUNTIF(W$6:W$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="X24" s="1">
-        <f>COUNTIF(X$6:X$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Y24" s="1">
-        <f>COUNTIF(Y$6:Y$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="Z24" s="1">
-        <f>COUNTIF(Z$6:Z$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA24" s="1">
-        <f>COUNTIF(AA$6:AA$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
-        <f>COUNTIF(AB$6:AB$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <f>COUNTIF(AC$6:AC$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AD24" s="1">
-        <f>COUNTIF(AD$6:AD$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>4</v>
       </c>
@@ -2681,119 +2719,119 @@
         <v>63</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:AE25" si="3">COUNTIF(C$6:C$20, "De acuerdo")</f>
+        <f t="shared" ref="C25:K25" si="6">COUNTIF(C$6:C$20, "De acuerdo")</f>
         <v>3</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L25" s="1">
-        <f>COUNTIF(L$6:L$20, "De acuerdo")</f>
+        <f t="shared" ref="L25:AD25" si="7">COUNTIF(L$6:L$20, "De acuerdo")</f>
         <v>1</v>
       </c>
       <c r="M25" s="1">
-        <f>COUNTIF(M$6:M$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="N25" s="1">
-        <f>COUNTIF(N$6:N$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="O25" s="1">
-        <f>COUNTIF(O$6:O$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="P25" s="1">
-        <f>COUNTIF(P$6:P$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="Q25" s="1">
-        <f>COUNTIF(Q$6:Q$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="R25" s="1">
-        <f>COUNTIF(R$6:R$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="S25" s="1">
-        <f>COUNTIF(S$6:S$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="T25" s="1">
-        <f>COUNTIF(T$6:T$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="U25" s="1">
-        <f>COUNTIF(U$6:U$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="V25" s="1">
-        <f>COUNTIF(V$6:V$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="W25" s="1">
-        <f>COUNTIF(W$6:W$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="X25" s="1">
-        <f>COUNTIF(X$6:X$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="Y25" s="1">
-        <f>COUNTIF(Y$6:Y$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="Z25" s="1">
-        <f>COUNTIF(Z$6:Z$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="AA25" s="1">
-        <f>COUNTIF(AA$6:AA$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AB25" s="1">
-        <f>COUNTIF(AB$6:AB$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AC25" s="1">
-        <f>COUNTIF(AC$6:AC$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="AD25" s="1">
-        <f>COUNTIF(AD$6:AD$20, "De acuerdo")</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -2801,115 +2839,115 @@
         <v>61</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ref="C26:AE26" si="4">COUNTIF(C$6:C$20, "Muy de acuerdo")</f>
+        <f t="shared" ref="C26:K26" si="8">COUNTIF(C$6:C$20, "Muy de acuerdo")</f>
         <v>9</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="L26" s="1">
-        <f>COUNTIF(L$6:L$20, "Muy de acuerdo")</f>
+        <f t="shared" ref="L26:AD26" si="9">COUNTIF(L$6:L$20, "Muy de acuerdo")</f>
         <v>11</v>
       </c>
       <c r="M26" s="1">
-        <f>COUNTIF(M$6:M$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="N26" s="1">
-        <f>COUNTIF(N$6:N$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="O26" s="1">
-        <f>COUNTIF(O$6:O$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="P26" s="1">
-        <f>COUNTIF(P$6:P$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="Q26" s="1">
-        <f>COUNTIF(Q$6:Q$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="R26" s="1">
-        <f>COUNTIF(R$6:R$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="S26" s="1">
-        <f>COUNTIF(S$6:S$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="T26" s="1">
-        <f>COUNTIF(T$6:T$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="U26" s="1">
-        <f>COUNTIF(U$6:U$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="V26" s="1">
-        <f>COUNTIF(V$6:V$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="W26" s="1">
-        <f>COUNTIF(W$6:W$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="X26" s="1">
-        <f>COUNTIF(X$6:X$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="Y26" s="1">
-        <f>COUNTIF(Y$6:Y$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z26" s="1">
-        <f>COUNTIF(Z$6:Z$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="AA26" s="1">
-        <f>COUNTIF(AA$6:AA$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="AB26" s="1">
-        <f>COUNTIF(AB$6:AB$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AC26" s="1">
-        <f>COUNTIF(AC$6:AC$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AD26" s="1">
-        <f>COUNTIF(AD$6:AD$20, "Muy de acuerdo")</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
     </row>
@@ -3038,764 +3076,823 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC61F3A-E8CF-4B7D-914B-02FFE3C1EE08}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AD2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f ca="1">COUNTIF(A$3:A$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <f ca="1">COUNTIF(B$3:B$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f ca="1">COUNTIF(C$3:C$18, "Muy en desacuerdo")</f>
+      <c r="A3" s="3">
+        <f t="shared" ref="A3:U7" ca="1" si="0">COUNTIF(A$3:A$18, "Muy en desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <f ca="1">COUNTIF(D$3:D$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <f ca="1">COUNTIF(E$3:E$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <f ca="1">COUNTIF(F$3:F$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <f ca="1">COUNTIF(G$3:G$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <f ca="1">COUNTIF(H$3:H$18, "Muy en desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <f ca="1">COUNTIF(I$3:I$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <f ca="1">COUNTIF(J$3:J$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <f ca="1">COUNTIF(K$3:K$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <f ca="1">COUNTIF(L$3:L$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <f ca="1">COUNTIF(M$3:M$18, "Muy en desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <f ca="1">COUNTIF(N$3:N$18, "Muy en desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="O3" s="1">
-        <f ca="1">COUNTIF(O$3:O$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <f ca="1">COUNTIF(P$3:P$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <f ca="1">COUNTIF(Q$3:Q$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <f>COUNTIF(R$3:R$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <f>COUNTIF(S$3:S$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <f>COUNTIF(T$3:T$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <f>COUNTIF(U$3:U$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Y3" s="1">
-        <f>COUNTIF(V$3:V$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="1">
-        <f>COUNTIF(W$3:W$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <f>COUNTIF(X$3:X$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <f>COUNTIF(Y$3:Y$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <f>COUNTIF(Z$3:Z$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="1">
-        <f>COUNTIF(AA$3:AA$18, "Muy en desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1">
-        <f>COUNTIF(AB$3:AB$18, "Muy en desacuerdo")</f>
+      <c r="D3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>15</v>
+      </c>
+      <c r="S3" s="6">
+        <v>15</v>
+      </c>
+      <c r="T3" s="6">
+        <v>15</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" ref="U3:AE3" ca="1" si="1">COUNTIF(U$6:U$20, "Muy en desacuerdo")</f>
+        <v>1</v>
+      </c>
+      <c r="V3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="W3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Y3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD3" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f ca="1">COUNTIF(A$3:A$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <f ca="1">COUNTIF(B$3:B$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <f ca="1">COUNTIF(C$3:C$18, "En desacuerdo")</f>
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:Q4" ca="1" si="2">COUNTIF(A$3:A$18, "En desacuerdo")</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
-      <c r="D4" s="1">
-        <f ca="1">COUNTIF(D$3:D$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <f ca="1">COUNTIF(E$3:E$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <f ca="1">COUNTIF(F$3:F$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <f ca="1">COUNTIF(G$3:G$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <f ca="1">COUNTIF(H$3:H$18, "En desacuerdo")</f>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
-      <c r="I4" s="1">
-        <f ca="1">COUNTIF(I$3:I$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <f ca="1">COUNTIF(J$3:J$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <f ca="1">COUNTIF(K$3:K$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <f ca="1">COUNTIF(L$3:L$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <f ca="1">COUNTIF(M$3:M$18, "En desacuerdo")</f>
+      <c r="I4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-      <c r="N4" s="1">
-        <f ca="1">COUNTIF(N$3:N$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <f ca="1">COUNTIF(O$3:O$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <f ca="1">COUNTIF(P$3:P$18, "En desacuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1">
-        <f ca="1">COUNTIF(Q$3:Q$18, "En desacuerdo")</f>
+      <c r="N4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-      <c r="U4" s="1">
-        <f>COUNTIF(R$3:R$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <f>COUNTIF(S$3:S$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="W4" s="1">
-        <f>COUNTIF(T$3:T$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="X4" s="1">
-        <f>COUNTIF(U$3:U$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="1">
-        <f>COUNTIF(V$3:V$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="1">
-        <f>COUNTIF(W$3:W$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="1">
-        <f>COUNTIF(X$3:X$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1">
-        <f>COUNTIF(Y$3:Y$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1">
-        <f>COUNTIF(Z$3:Z$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="1">
-        <f>COUNTIF(AA$3:AA$18, "En desacuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="1">
-        <f>COUNTIF(AB$3:AB$18, "En desacuerdo")</f>
+      <c r="R4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" ref="U4:AE4" ca="1" si="3">COUNTIF(U$6:U$20, "En desacuerdo")</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="X4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="Z4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AD4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f ca="1">COUNTIF(A$3:A$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="A5" s="3">
+        <f t="shared" ref="A5:Q5" ca="1" si="4">COUNTIF(A$3:A$18, "Ni en desacuerdo ni de acuerdo")</f>
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <f ca="1">COUNTIF(B$3:B$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <f ca="1">COUNTIF(C$3:C$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <f ca="1">COUNTIF(D$3:D$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>5</v>
       </c>
-      <c r="E5" s="1">
-        <f ca="1">COUNTIF(E$3:E$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="E5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
-      <c r="F5" s="1">
-        <f ca="1">COUNTIF(F$3:F$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="F5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
-      <c r="G5" s="1">
-        <f ca="1">COUNTIF(G$3:G$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="G5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
-      <c r="H5" s="1">
-        <f ca="1">COUNTIF(H$3:H$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <f ca="1">COUNTIF(I$3:I$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="H5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
-      <c r="J5" s="1">
-        <f ca="1">COUNTIF(J$3:J$18, "Ni en desacuerdo ni de acuerdo")</f>
+      <c r="J5" s="3">
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
-      <c r="K5" s="1">
-        <f ca="1">COUNTIF(K$3:K$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <f ca="1">COUNTIF(L$3:L$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <f ca="1">COUNTIF(M$3:M$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="N5" s="1">
-        <f ca="1">COUNTIF(N$3:N$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <f ca="1">COUNTIF(O$3:O$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
-        <f ca="1">COUNTIF(P$3:P$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1">
-        <f ca="1">COUNTIF(Q$3:Q$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="U5" s="1">
-        <f>COUNTIF(R$3:R$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="1">
-        <f>COUNTIF(S$3:S$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="W5" s="1">
-        <f>COUNTIF(T$3:T$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="X5" s="1">
-        <f>COUNTIF(U$3:U$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="1">
-        <f>COUNTIF(V$3:V$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="1">
-        <f>COUNTIF(W$3:W$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1">
-        <f>COUNTIF(X$3:X$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1">
-        <f>COUNTIF(Y$3:Y$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1">
-        <f>COUNTIF(Z$3:Z$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="1">
-        <f>COUNTIF(AA$3:AA$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="1">
-        <f>COUNTIF(AB$3:AB$18, "Ni en desacuerdo ni de acuerdo")</f>
-        <v>0</v>
+      <c r="K5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="P5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" ref="U5:AE5" ca="1" si="5">COUNTIF(U$6:U$20, "Ni en desacuerdo ni de acuerdo")</f>
+        <v>1</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Z5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AE5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f ca="1">COUNTIF(A$3:A$18, "De acuerdo")</f>
+      <c r="A6" s="3">
+        <f t="shared" ref="A6:Q6" ca="1" si="6">COUNTIF(A$3:A$18, "De acuerdo")</f>
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <f ca="1">COUNTIF(B$3:B$18, "De acuerdo")</f>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <f ca="1">COUNTIF(C$3:C$18, "De acuerdo")</f>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="D6" s="1">
-        <f ca="1">COUNTIF(D$3:D$18, "De acuerdo")</f>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>6</v>
       </c>
-      <c r="E6" s="1">
-        <f ca="1">COUNTIF(E$3:E$18, "De acuerdo")</f>
+      <c r="E6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="F6" s="1">
-        <f ca="1">COUNTIF(F$3:F$18, "De acuerdo")</f>
+      <c r="F6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>9</v>
       </c>
-      <c r="G6" s="1">
-        <f ca="1">COUNTIF(G$3:G$18, "De acuerdo")</f>
+      <c r="G6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>8</v>
       </c>
-      <c r="H6" s="1">
-        <f ca="1">COUNTIF(H$3:H$18, "De acuerdo")</f>
+      <c r="H6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="I6" s="1">
-        <f ca="1">COUNTIF(I$3:I$18, "De acuerdo")</f>
+      <c r="I6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="J6" s="1">
-        <f ca="1">COUNTIF(J$3:J$18, "De acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
-        <f ca="1">COUNTIF(K$3:K$18, "De acuerdo")</f>
+      <c r="J6" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="L6" s="1">
-        <f ca="1">COUNTIF(L$3:L$18, "De acuerdo")</f>
+      <c r="L6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>5</v>
       </c>
-      <c r="M6" s="1">
-        <f ca="1">COUNTIF(M$3:M$18, "De acuerdo")</f>
+      <c r="M6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
-      <c r="N6" s="1">
-        <f ca="1">COUNTIF(N$3:N$18, "De acuerdo")</f>
+      <c r="N6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
-      <c r="O6" s="1">
-        <f ca="1">COUNTIF(O$3:O$18, "De acuerdo")</f>
+      <c r="O6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="P6" s="1">
-        <f ca="1">COUNTIF(P$3:P$18, "De acuerdo")</f>
+      <c r="P6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>7</v>
       </c>
-      <c r="Q6" s="1">
-        <f ca="1">COUNTIF(Q$3:Q$18, "De acuerdo")</f>
+      <c r="Q6" s="3">
+        <f t="shared" ca="1" si="6"/>
         <v>2</v>
       </c>
-      <c r="U6" s="1">
-        <f>COUNTIF(R$3:R$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="V6" s="1">
-        <f>COUNTIF(S$3:S$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="1">
-        <f>COUNTIF(T$3:T$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="X6" s="1">
-        <f>COUNTIF(U$3:U$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="1">
-        <f>COUNTIF(V$3:V$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="1">
-        <f>COUNTIF(W$3:W$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="1">
-        <f>COUNTIF(X$3:X$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="1">
-        <f>COUNTIF(Y$3:Y$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1">
-        <f>COUNTIF(Z$3:Z$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AD6" s="1">
-        <f>COUNTIF(AA$3:AA$18, "De acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="1">
-        <f>COUNTIF(AB$3:AB$18, "De acuerdo")</f>
-        <v>0</v>
+      <c r="R6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" ref="U6:AE6" ca="1" si="7">COUNTIF(U$6:U$20, "De acuerdo")</f>
+        <v>3</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="W6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="X6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Z6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AA6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="AB6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="AD6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="AE6" s="3">
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <f ca="1">COUNTIF(A$3:A$18, "Muy de acuerdo")</f>
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:Q7" ca="1" si="8">COUNTIF(A$3:A$18, "Muy de acuerdo")</f>
         <v>9</v>
       </c>
-      <c r="B7" s="1">
-        <f ca="1">COUNTIF(B$3:B$18, "Muy de acuerdo")</f>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="C7" s="1">
-        <f ca="1">COUNTIF(C$3:C$18, "Muy de acuerdo")</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <f ca="1">COUNTIF(D$3:D$18, "Muy de acuerdo")</f>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
-      <c r="E7" s="1">
-        <f ca="1">COUNTIF(E$3:E$18, "Muy de acuerdo")</f>
+      <c r="E7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
-      <c r="F7" s="1">
-        <f ca="1">COUNTIF(F$3:F$18, "Muy de acuerdo")</f>
+      <c r="F7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
-      <c r="G7" s="1">
-        <f ca="1">COUNTIF(G$3:G$18, "Muy de acuerdo")</f>
+      <c r="G7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>2</v>
       </c>
-      <c r="H7" s="1">
-        <f ca="1">COUNTIF(H$3:H$18, "Muy de acuerdo")</f>
+      <c r="H7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>7</v>
       </c>
-      <c r="I7" s="1">
-        <f ca="1">COUNTIF(I$3:I$18, "Muy de acuerdo")</f>
+      <c r="I7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="J7" s="1">
-        <f ca="1">COUNTIF(J$3:J$18, "Muy de acuerdo")</f>
+      <c r="J7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>11</v>
       </c>
-      <c r="K7" s="1">
-        <f ca="1">COUNTIF(K$3:K$18, "Muy de acuerdo")</f>
+      <c r="K7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="L7" s="1">
-        <f ca="1">COUNTIF(L$3:L$18, "Muy de acuerdo")</f>
+      <c r="L7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="M7" s="1">
-        <f ca="1">COUNTIF(M$3:M$18, "Muy de acuerdo")</f>
+      <c r="M7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
-      <c r="N7" s="1">
-        <f ca="1">COUNTIF(N$3:N$18, "Muy de acuerdo")</f>
+      <c r="N7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>9</v>
       </c>
-      <c r="O7" s="1">
-        <f ca="1">COUNTIF(O$3:O$18, "Muy de acuerdo")</f>
+      <c r="O7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>7</v>
       </c>
-      <c r="P7" s="1">
-        <f ca="1">COUNTIF(P$3:P$18, "Muy de acuerdo")</f>
+      <c r="P7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>6</v>
       </c>
-      <c r="Q7" s="1">
-        <f ca="1">COUNTIF(Q$3:Q$18, "Muy de acuerdo")</f>
+      <c r="Q7" s="3">
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
-      <c r="U7" s="1">
-        <f>COUNTIF(R$3:R$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="1">
-        <f>COUNTIF(S$3:S$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="W7" s="1">
-        <f>COUNTIF(T$3:T$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="X7" s="1">
-        <f>COUNTIF(U$3:U$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="1">
-        <f>COUNTIF(V$3:V$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="1">
-        <f>COUNTIF(W$3:W$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="1">
-        <f>COUNTIF(X$3:X$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="1">
-        <f>COUNTIF(Y$3:Y$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="1">
-        <f>COUNTIF(Z$3:Z$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AD7" s="1">
-        <f>COUNTIF(AA$3:AA$18, "Muy de acuerdo")</f>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="1">
-        <f>COUNTIF(AB$3:AB$18, "Muy de acuerdo")</f>
-        <v>0</v>
+      <c r="R7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" ref="U7:AE7" ca="1" si="9">COUNTIF(U$6:U$20, "Muy de acuerdo")</f>
+        <v>10</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="W7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="X7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="Z7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="AB7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="AD7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" ca="1" si="9"/>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -4101,5 +4198,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>